<commit_message>
Create test case#6 and #7
</commit_message>
<xml_diff>
--- a/POM_Practice/src/test/resources/testData/TestData.xlsx
+++ b/POM_Practice/src/test/resources/testData/TestData.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9C027906-CDF0-454F-AFF1-ABF93EE6A8A3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\POM_Practice\POM_Practice\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1DDD5D-2C8B-4814-8B55-73390A2B1D78}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="29070" windowHeight="16500" xr2:uid="{2143D607-5BED-49F2-A1E3-D9749D359B17}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2143D607-5BED-49F2-A1E3-D9749D359B17}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="18">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -68,26 +72,32 @@
     <t>Standard</t>
   </si>
   <si>
-    <t>1 - One</t>
-  </si>
-  <si>
     <t>25/02/2019</t>
   </si>
   <si>
     <t>26/02/2019</t>
+  </si>
+  <si>
+    <t>3 - Three</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -110,8 +120,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,7 +440,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,17 +504,18 @@
       <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>